<commit_message>
Evaluations from varying SP
</commit_message>
<xml_diff>
--- a/P-R_meanDetectionScore_15SP_chart.xlsx
+++ b/P-R_meanDetectionScore_15SP_chart.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="16275" windowHeight="7740"/>
+    <workbookView xWindow="12300" yWindow="1080" windowWidth="16275" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="P-R_meanDetectionScore" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -558,10 +558,10 @@
           <c:order val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>'P-R_meanDetectionScore'!$A$1:$A$19</c:f>
+              <c:f>'P-R_meanDetectionScore'!$A$1:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0.93976000000000004</c:v>
                 </c:pt>
@@ -615,19 +615,16 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1.2048E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'P-R_meanDetectionScore'!$B$1:$B$19</c:f>
+              <c:f>'P-R_meanDetectionScore'!$B$1:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>8.1504999999999994E-2</c:v>
                 </c:pt>
@@ -681,41 +678,37 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.66666999999999998</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="86311680"/>
-        <c:axId val="85453824"/>
+        <c:axId val="99033088"/>
+        <c:axId val="99034624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86311680"/>
+        <c:axId val="99033088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85453824"/>
+        <c:crossAx val="99034624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85453824"/>
+        <c:axId val="99034624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86311680"/>
+        <c:crossAx val="99033088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -728,7 +721,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -739,19 +732,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1057,7 +1050,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B19"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>